<commit_message>
up tim hieu co ban ve hashtag
</commit_message>
<xml_diff>
--- a/04. Ke Hoach/03. Ke hoach ca nhan/Sang/TodoList_Sang.xlsx
+++ b/04. Ke Hoach/03. Ke hoach ca nhan/Sang/TodoList_Sang.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>KẾ HOẠCH LÀM VIỆC  GIAI ĐOẠN 1</t>
   </si>
@@ -100,18 +100,12 @@
     <t>Đã hoàn thành</t>
   </si>
   <si>
-    <t>Chưa hoàn thành thời gian</t>
-  </si>
-  <si>
     <t>Cần trao dồi và bổ xung thêm</t>
   </si>
   <si>
     <t>Tìm hiểu thuật toán tăng tương tác trong istagram</t>
   </si>
   <si>
-    <t>Tìm hiểu về Hashtag</t>
-  </si>
-  <si>
     <t>Tìm hiểu sơ qua về số liệu thống kê trong instagram</t>
   </si>
   <si>
@@ -122,6 +116,9 @@
   </si>
   <si>
     <t>Người lập: Nguyễn Văn Sang</t>
+  </si>
+  <si>
+    <t>Tìm hiểu cơ bản về Hashtag</t>
   </si>
 </sst>
 </file>
@@ -394,131 +391,134 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -543,9 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,14 +837,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -855,458 +852,458 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="H3" s="12" t="s">
+      <c r="H3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44" t="s">
+      <c r="E5" s="11"/>
+      <c r="F5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="44"/>
-      <c r="H5" s="44" t="s">
+      <c r="G5" s="11"/>
+      <c r="H5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="44"/>
-      <c r="N5" s="50" t="s">
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="51"/>
-      <c r="P5" s="44" t="s">
+      <c r="O5" s="15"/>
+      <c r="P5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="Q5" s="44"/>
-      <c r="R5" s="44"/>
-      <c r="S5" s="44"/>
-      <c r="T5" s="44"/>
-      <c r="U5" s="44" t="s">
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="V5" s="44"/>
-      <c r="W5" s="44"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>1</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B6" s="24">
         <v>43690</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23">
+      <c r="C6" s="24"/>
+      <c r="D6" s="24">
         <v>43694</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="43">
+      <c r="E6" s="24"/>
+      <c r="F6" s="12">
         <v>5</v>
       </c>
-      <c r="G6" s="43"/>
-      <c r="H6" s="49" t="s">
+      <c r="G6" s="12"/>
+      <c r="H6" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="38"/>
-      <c r="P6" s="43"/>
-      <c r="Q6" s="43"/>
-      <c r="R6" s="43"/>
-      <c r="S6" s="43"/>
-      <c r="T6" s="43"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="43"/>
-      <c r="W6" s="43"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12"/>
+      <c r="W6" s="12"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="42">
         <v>2</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="44">
         <v>43690</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="15">
+      <c r="C7" s="45"/>
+      <c r="D7" s="44">
         <v>43690</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="19">
+      <c r="E7" s="45"/>
+      <c r="F7" s="48">
         <v>1</v>
       </c>
-      <c r="G7" s="20"/>
-      <c r="H7" s="45" t="s">
+      <c r="G7" s="49"/>
+      <c r="H7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="31"/>
-      <c r="T7" s="32"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="20"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="45"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="45"/>
-      <c r="M8" s="45"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="34"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="34"/>
-      <c r="T8" s="35"/>
-      <c r="U8" s="33"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="35"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="23"/>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="23">
+      <c r="B9" s="24">
         <v>43690</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23">
+      <c r="C9" s="24"/>
+      <c r="D9" s="24">
         <v>43692</v>
       </c>
-      <c r="E9" s="23"/>
-      <c r="F9" s="43">
+      <c r="E9" s="24"/>
+      <c r="F9" s="12">
         <v>2</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="48" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="38"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="37"/>
-      <c r="R9" s="37"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="38"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="38"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="39"/>
+      <c r="R9" s="39"/>
+      <c r="S9" s="39"/>
+      <c r="T9" s="32"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="39"/>
+      <c r="W9" s="32"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>4</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="35">
         <v>43695</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24">
+      <c r="C10" s="35"/>
+      <c r="D10" s="35">
         <v>43695</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="29">
+      <c r="E10" s="35"/>
+      <c r="F10" s="37">
         <v>4</v>
       </c>
-      <c r="G10" s="29"/>
-      <c r="H10" s="45" t="s">
+      <c r="G10" s="37"/>
+      <c r="H10" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="45"/>
-      <c r="J10" s="45"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="45"/>
-      <c r="M10" s="45"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="40"/>
-      <c r="R10" s="40"/>
-      <c r="S10" s="40"/>
-      <c r="T10" s="41"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="40"/>
-      <c r="W10" s="41"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="38"/>
+      <c r="T10" s="34"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="38"/>
+      <c r="W10" s="34"/>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>5</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43">
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12">
         <v>0.75</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="46" t="s">
+      <c r="G11" s="12"/>
+      <c r="H11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="46"/>
-      <c r="J11" s="46"/>
-      <c r="K11" s="46"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="46"/>
-      <c r="N11" s="36"/>
-      <c r="O11" s="38"/>
-      <c r="P11" s="36"/>
-      <c r="Q11" s="37"/>
-      <c r="R11" s="37"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="38"/>
-      <c r="U11" s="36"/>
-      <c r="V11" s="37"/>
-      <c r="W11" s="38"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="32"/>
+      <c r="P11" s="31"/>
+      <c r="Q11" s="39"/>
+      <c r="R11" s="39"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="32"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="39"/>
+      <c r="W11" s="32"/>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12" s="13">
+      <c r="A12" s="42">
         <v>6</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="42">
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="36">
         <v>45</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="45" t="s">
+      <c r="G12" s="36"/>
+      <c r="H12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="45"/>
-      <c r="M12" s="45"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="32"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="31"/>
-      <c r="R12" s="31"/>
-      <c r="S12" s="31"/>
-      <c r="T12" s="32"/>
-      <c r="U12" s="30"/>
-      <c r="V12" s="31"/>
-      <c r="W12" s="32"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16"/>
+      <c r="M12" s="16"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="19"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="19"/>
+      <c r="W12" s="20"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="45"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="35"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="34"/>
-      <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
-      <c r="T13" s="35"/>
-      <c r="U13" s="33"/>
-      <c r="V13" s="34"/>
-      <c r="W13" s="35"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="22"/>
+      <c r="S13" s="22"/>
+      <c r="T13" s="23"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="22"/>
+      <c r="W13" s="23"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>7</v>
       </c>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="43">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="12">
         <v>30</v>
       </c>
-      <c r="G14" s="43"/>
-      <c r="H14" s="46" t="s">
+      <c r="G14" s="12"/>
+      <c r="H14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="46"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="38"/>
-      <c r="P14" s="36"/>
-      <c r="Q14" s="37"/>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="38"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="38"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="32"/>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>8</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="29">
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="35"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="37">
         <v>30</v>
       </c>
-      <c r="G15" s="29"/>
-      <c r="H15" s="47" t="s">
+      <c r="G15" s="37"/>
+      <c r="H15" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="47"/>
-      <c r="L15" s="47"/>
-      <c r="M15" s="47"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="41"/>
-      <c r="U15" s="39"/>
-      <c r="V15" s="40"/>
-      <c r="W15" s="41"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="34"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="38"/>
+      <c r="T15" s="34"/>
+      <c r="U15" s="33"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="34"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>9</v>
       </c>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="43">
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="12">
         <v>30</v>
       </c>
-      <c r="G16" s="43"/>
-      <c r="H16" s="46" t="s">
+      <c r="G16" s="12"/>
+      <c r="H16" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="38"/>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="37"/>
-      <c r="R16" s="37"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="38"/>
-      <c r="U16" s="36"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="38"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="31"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="39"/>
+      <c r="W16" s="32"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="13">
+      <c r="A17" s="42">
         <v>10</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="42">
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="36">
         <v>20</v>
       </c>
-      <c r="G17" s="42"/>
-      <c r="H17" s="45" t="s">
+      <c r="G17" s="36"/>
+      <c r="H17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="I17" s="45"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="45"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="30"/>
-      <c r="O17" s="32"/>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="32"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="32"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
+      <c r="N17" s="18"/>
+      <c r="O17" s="20"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="20"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="20"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="45"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="33"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="34"/>
-      <c r="R18" s="34"/>
-      <c r="S18" s="34"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="33"/>
-      <c r="V18" s="34"/>
-      <c r="W18" s="35"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="21"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="23"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
@@ -1319,34 +1316,43 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="H5:M5"/>
-    <mergeCell ref="P5:T5"/>
-    <mergeCell ref="U5:W5"/>
-    <mergeCell ref="P6:T6"/>
-    <mergeCell ref="U6:W6"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="H7:M8"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="H10:M10"/>
-    <mergeCell ref="P7:T8"/>
-    <mergeCell ref="U7:W8"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="H17:M18"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="H11:M11"/>
-    <mergeCell ref="H12:M13"/>
-    <mergeCell ref="H14:M14"/>
-    <mergeCell ref="H16:M16"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B7:C8"/>
+    <mergeCell ref="D7:E8"/>
+    <mergeCell ref="F7:G8"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="U12:W13"/>
+    <mergeCell ref="U17:W18"/>
+    <mergeCell ref="U9:W9"/>
+    <mergeCell ref="U10:W10"/>
+    <mergeCell ref="U11:W11"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="U15:W15"/>
+    <mergeCell ref="U16:W16"/>
+    <mergeCell ref="P15:T15"/>
+    <mergeCell ref="P16:T16"/>
+    <mergeCell ref="P12:T13"/>
+    <mergeCell ref="P17:T18"/>
+    <mergeCell ref="P9:T9"/>
+    <mergeCell ref="P10:T10"/>
+    <mergeCell ref="P11:T11"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="N12:O13"/>
     <mergeCell ref="N17:O18"/>
     <mergeCell ref="D12:E13"/>
     <mergeCell ref="N6:O6"/>
@@ -1363,43 +1369,34 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="F17:G18"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="N12:O13"/>
-    <mergeCell ref="P15:T15"/>
-    <mergeCell ref="P16:T16"/>
-    <mergeCell ref="P12:T13"/>
-    <mergeCell ref="P17:T18"/>
-    <mergeCell ref="P9:T9"/>
-    <mergeCell ref="P10:T10"/>
-    <mergeCell ref="P11:T11"/>
-    <mergeCell ref="P14:T14"/>
-    <mergeCell ref="U12:W13"/>
-    <mergeCell ref="U17:W18"/>
-    <mergeCell ref="U9:W9"/>
-    <mergeCell ref="U10:W10"/>
-    <mergeCell ref="U11:W11"/>
-    <mergeCell ref="U14:W14"/>
-    <mergeCell ref="U15:W15"/>
-    <mergeCell ref="U16:W16"/>
-    <mergeCell ref="H1:M1"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B7:C8"/>
-    <mergeCell ref="D7:E8"/>
-    <mergeCell ref="F7:G8"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C18"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="H17:M18"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="H11:M11"/>
+    <mergeCell ref="H12:M13"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="H16:M16"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="H7:M8"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="H10:M10"/>
+    <mergeCell ref="P7:T8"/>
+    <mergeCell ref="U7:W8"/>
+    <mergeCell ref="H5:M5"/>
+    <mergeCell ref="P5:T5"/>
+    <mergeCell ref="U5:W5"/>
+    <mergeCell ref="P6:T6"/>
+    <mergeCell ref="U6:W6"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1411,7 +1408,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1427,145 +1424,149 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44" t="s">
+      <c r="E4" s="11"/>
+      <c r="F4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44" t="s">
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="44"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="44" t="s">
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="R4" s="44"/>
-      <c r="S4" s="44"/>
-      <c r="T4" s="44"/>
-      <c r="U4" s="44"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="54">
         <v>43767</v>
       </c>
-      <c r="C5" s="54"/>
-      <c r="D5" s="60">
+      <c r="C5" s="55"/>
+      <c r="D5" s="61">
         <v>2</v>
       </c>
-      <c r="E5" s="60"/>
-      <c r="F5" s="59" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="60" t="s">
+      <c r="E5" s="61"/>
+      <c r="F5" s="60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="60"/>
+      <c r="H5" s="60"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="60"/>
+      <c r="K5" s="60"/>
+      <c r="L5" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="60"/>
-      <c r="N5" s="60"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="60" t="s">
-        <v>27</v>
-      </c>
-      <c r="R5" s="60"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="60"/>
-      <c r="U5" s="60"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="R5" s="61"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="61"/>
+      <c r="U5" s="61"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>2</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="56"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="57"/>
       <c r="D6" s="52">
         <v>1</v>
       </c>
       <c r="E6" s="52"/>
-      <c r="F6" s="61" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="52" t="s">
+      <c r="F6" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="52"/>
-      <c r="N6" s="52"/>
-      <c r="O6" s="52"/>
-      <c r="P6" s="52"/>
-      <c r="Q6" s="52"/>
-      <c r="R6" s="52"/>
-      <c r="S6" s="52"/>
-      <c r="T6" s="52"/>
-      <c r="U6" s="52"/>
+      <c r="R6" s="61"/>
+      <c r="S6" s="61"/>
+      <c r="T6" s="61"/>
+      <c r="U6" s="61"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>3</v>
       </c>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="60">
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="61">
         <v>0.5</v>
       </c>
-      <c r="E7" s="60"/>
-      <c r="F7" s="59" t="s">
+      <c r="E7" s="61"/>
+      <c r="F7" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="R7" s="60"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="60"/>
-      <c r="U7" s="60"/>
+      <c r="R7" s="61"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="61"/>
+      <c r="U7" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="L7:P7"/>
+    <mergeCell ref="Q7:U7"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:K6"/>
     <mergeCell ref="L6:P6"/>
@@ -1582,8 +1583,6 @@
     <mergeCell ref="Q5:U5"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:K7"/>
-    <mergeCell ref="L7:P7"/>
-    <mergeCell ref="Q7:U7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>